<commit_message>
remove softdeletes, artisan make seeders, implement delete book
</commit_message>
<xml_diff>
--- a/public/books.xlsx
+++ b/public/books.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Θεματική</t>
   </si>
@@ -49,45 +49,6 @@
   </si>
   <si>
     <t>Εκδότης*</t>
-  </si>
-  <si>
-    <t>Εισαγωγή στην ψυχανάλυση</t>
-  </si>
-  <si>
-    <t>Sigmun Freud</t>
-  </si>
-  <si>
-    <t>Νίκας</t>
-  </si>
-  <si>
-    <t>Ψυχολογία</t>
-  </si>
-  <si>
-    <t>Αθήνα</t>
-  </si>
-  <si>
-    <t>Αγορά</t>
-  </si>
-  <si>
-    <t>Καινούριο</t>
-  </si>
-  <si>
-    <t>Ο Ξένος</t>
-  </si>
-  <si>
-    <t>Albert Camus</t>
-  </si>
-  <si>
-    <t>Καστανιώτης</t>
-  </si>
-  <si>
-    <t>Ξένη Λογοτεχνία</t>
-  </si>
-  <si>
-    <t>Δωρεά</t>
-  </si>
-  <si>
-    <t>Μεταχειρισμένο</t>
   </si>
 </sst>
 </file>
@@ -453,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -508,76 +469,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2">
-        <v>98</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2">
-        <v>2017</v>
-      </c>
-      <c r="H2">
-        <v>632</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2">
-        <v>2022</v>
-      </c>
-      <c r="K2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3">
-        <v>99</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3">
-        <v>1990</v>
-      </c>
-      <c r="H3">
-        <v>120</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3">
-        <v>2021</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
read uploading books file
</commit_message>
<xml_diff>
--- a/public/books.xlsx
+++ b/public/books.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Θεματική</t>
   </si>
@@ -49,45 +49,6 @@
   </si>
   <si>
     <t>Εκδότης*</t>
-  </si>
-  <si>
-    <t>Εισαγωγή στην ψυχανάλυση</t>
-  </si>
-  <si>
-    <t>Sigmun Freud</t>
-  </si>
-  <si>
-    <t>Νίκας</t>
-  </si>
-  <si>
-    <t>Ψυχολογία</t>
-  </si>
-  <si>
-    <t>Αθήνα</t>
-  </si>
-  <si>
-    <t>Αγορά</t>
-  </si>
-  <si>
-    <t>Καινούριο</t>
-  </si>
-  <si>
-    <t>Ο Ξένος</t>
-  </si>
-  <si>
-    <t>Albert Camus</t>
-  </si>
-  <si>
-    <t>Καστανιώτης</t>
-  </si>
-  <si>
-    <t>Ξένη Λογοτεχνία</t>
-  </si>
-  <si>
-    <t>Δωρεά</t>
-  </si>
-  <si>
-    <t>Μεταχειρισμένο</t>
   </si>
 </sst>
 </file>
@@ -453,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -508,76 +469,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2">
-        <v>98</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2">
-        <v>2017</v>
-      </c>
-      <c r="H2">
-        <v>632</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2">
-        <v>2022</v>
-      </c>
-      <c r="K2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3">
-        <v>99</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3">
-        <v>1990</v>
-      </c>
-      <c r="H3">
-        <v>120</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3">
-        <v>2021</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>